<commit_message>
Back-end code task design and division of labor, overall flowchart drawing
</commit_message>
<xml_diff>
--- a/workdivideandstorage.xlsx
+++ b/workdivideandstorage.xlsx
@@ -8,17 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\VSCode\CUHK-vscode\pre设计\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9EAC4F6-AC90-4A4A-B9DB-E43D288BE15E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60697F5D-20DB-4A55-8F67-F6B56BDFC4AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-12" yWindow="48" windowWidth="15300" windowHeight="10824" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="分工" sheetId="1" r:id="rId1"/>
     <sheet name="题目类型" sheetId="3" r:id="rId2"/>
-    <sheet name="题目表1" sheetId="2" r:id="rId3"/>
+    <sheet name="Basic python" sheetId="2" r:id="rId3"/>
     <sheet name="题目表2" sheetId="4" r:id="rId4"/>
-    <sheet name="题目表n" sheetId="5" r:id="rId5"/>
-    <sheet name="答案" sheetId="6" r:id="rId6"/>
+    <sheet name="题目表3" sheetId="5" r:id="rId5"/>
+    <sheet name="题目表4" sheetId="7" r:id="rId6"/>
+    <sheet name="题目表5" sheetId="8" r:id="rId7"/>
+    <sheet name="答案" sheetId="6" r:id="rId8"/>
+    <sheet name="user" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="120">
   <si>
     <t>功能</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -108,18 +111,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>序号</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>题目</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>XXXX</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>类型</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -136,50 +131,115 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>选项1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>选项2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>XXX</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>选项3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>题号</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>答案</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>A</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>测试</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ABC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>题号（唯一）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>代码作答</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>判断</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>字符串是一个连续的字符序列，哪个选项可以实现打印字符信息的换行？</t>
+  </si>
+  <si>
+    <t>使用"\换行"</t>
+  </si>
+  <si>
+    <t>使用转义符\\</t>
+  </si>
+  <si>
+    <t>使用空格</t>
+  </si>
+  <si>
+    <t>val=pow(2, 1000)，使用一行代码返回val结果的长度值。</t>
+  </si>
+  <si>
+    <t>len(val)</t>
+  </si>
+  <si>
+    <t>len(pow(2, 1000))</t>
+  </si>
+  <si>
+    <t>len(str(val))</t>
+  </si>
+  <si>
+    <t>以上均不正确</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>哪个选项是下面代码的执行结果？name="Python语言程序设计课程"
+print(name[0], name[2:-2], name[-1])</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>P  thon语言程序设计  程</t>
+  </si>
+  <si>
+    <t>P  thon语言程序设计  课</t>
+  </si>
+  <si>
+    <t>P  thon语言程序设计课  程</t>
+  </si>
+  <si>
+    <t>P  thon语言程序设计课  课</t>
+  </si>
+  <si>
+    <t>请选出以下正确的选项</t>
+  </si>
+  <si>
+    <t>is可以判断数值是否相等</t>
+  </si>
+  <si>
+    <t>*arg：会把位置参数转化为tuple</t>
+  </si>
+  <si>
+    <t>浅拷贝指拷贝数据集合的所有层</t>
+  </si>
+  <si>
+    <t>布尔值为False的常见值有0, [] , () , {} , '' , False , None</t>
+  </si>
+  <si>
+    <t>求结果：v = dict.fromkeys(['k1','k2'],[])
+v['k1'].append(666)
+print(v)
+v['k1'] = 777
+print(v)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{'k1':[666],'k2':[]}， {'k1':777,'k2':[]}</t>
+  </si>
+  <si>
+    <t>{'k1':[666],'k2':[666]}， {'k1':777,'k2':[777]}</t>
+  </si>
+  <si>
+    <t>{'k1':[666],'k2':[]}， {'k1':666,'k2':[666]}</t>
+  </si>
+  <si>
+    <t>{'k1':[666],'k2':[666]}， {'k1':777,'k2':[666]}</t>
+  </si>
+  <si>
+    <t>如何实现 "1,2,3" 变成 ['1','2','3'] ?</t>
+  </si>
+  <si>
+    <t>写一个程序可以从列表中筛选出每个元素出现的次数,然后统计在新的一个字典my_dict中,键为元素名,值为出现的次数。lista=[2,  6, 18, 19, 17,  2, 12,  1,  1, 16,  9,  1,  3,  5,  5,  0, 17, 0,  2, 17]  
+Expected Output:  
+{2: 3, 6: 1, 18: 1, 19: 1, 17: 3, 12: 1, 1: 3, 16: 1, 9: 1, 3: 1, 5: 2, 0: 2}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">判断下列逻辑语句的True or False.1 &gt; 1 or 3 &lt; 4 or 4 &gt; 5 and 2 &gt; 1 and 9 &gt; 8 or 7 &lt; 6  </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>B</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -189,6 +249,238 @@
   </si>
   <si>
     <t>D</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>使用\n</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>判断下列逻辑语句的True or False.not 2 &gt; 1 and 3 &lt; 4 or 4 &gt; 5 and 2 &gt; 1 and 9 &gt; 8 or 7 &lt; 6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在循环中continue语句的作用是跳出当前循环</t>
+  </si>
+  <si>
+    <t>循环语句 for i in range(6,-4,-2):中，循环执行__次，循环变量的终值应当为__</t>
+  </si>
+  <si>
+    <t>6，-4</t>
+  </si>
+  <si>
+    <t>6，-2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5，-4</t>
+  </si>
+  <si>
+    <t>5，-2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>运行下列代码，最终i的值为__。i=0
+lst=[1,2,3,4]
+for x in lst:
+     x=int(x)
+     i=i+x</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表达式 5 if 5&gt;6 else (6 if 3&gt;2 else 5)的值为____</t>
+  </si>
+  <si>
+    <t>求1-100的所有数的和（要求输出“从1到100所有数的总和为【结果】”）expected output：从1到100所有数的总和为5050</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Python中定义函数时不需要声明函数参数的类型</t>
+  </si>
+  <si>
+    <t>定义阶段实参和形参无关，只有调用阶段实参的内存地址才会绑定给形参</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>名称空间把栈区名字分为内置名称空间,全局名称空间,局部名称空间三类</t>
+  </si>
+  <si>
+    <t>以下关于函数参数的描述，正确的是：</t>
+  </si>
+  <si>
+    <t>调用函数时，按参数名称传递的参数，要按照定义顺序进行传递</t>
+  </si>
+  <si>
+    <t>定义函数可选参数的时候，不限制可选参数在参数列表中的位置</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>函数在定义时可以不指定可选参数的默认值，调用函数的时候再传入参数</t>
+  </si>
+  <si>
+    <t>在一个函数内部定义的变量，到另一个函数中不能引用</t>
+  </si>
+  <si>
+    <t>关于基本输入输出函数的描述，错误的选项是：</t>
+  </si>
+  <si>
+    <t>print()函数的参数可以是一个函数，执行结果是显示函数返回的值</t>
+  </si>
+  <si>
+    <t>eval()函数的参数是“3*4”的时候，返回的值是整数“12”</t>
+  </si>
+  <si>
+    <t>当用户输入一个整数“6”的时候，input()函数返回的也是整数“6”</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>当print()函数输出多个变量的时候，可以用逗号分隔多个变量名</t>
+  </si>
+  <si>
+    <t>以下程序的输出结果是：L = []
+x = 3
+def pri_val(x):
+	L.append(x)
+x = 5
+pri_val(x)
+print('L = {}, x = {}'.format(L, x))</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>L = 3, x = 3</t>
+  </si>
+  <si>
+    <t>L = 3, x = 5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>L = [3], x = 5</t>
+  </si>
+  <si>
+    <t>L = [3], x = 3</t>
+  </si>
+  <si>
+    <t>请书写一个函数，接受两个数字参数并返回较大的那个数字</t>
+  </si>
+  <si>
+    <t>plt.xlim() 显示的是x轴的作图范围，而 plt.xticks() 表达的是x轴的刻度内容的范围</t>
+  </si>
+  <si>
+    <t>matplotlib作图时坐标轴数字可随意设置，不用增加额外的代码</t>
+  </si>
+  <si>
+    <t>matplotlib作图可以实现以下哪些操作？</t>
+  </si>
+  <si>
+    <t>以下两种写法是等价的：①ax=plt.subplot(2,2,1)
+②ax=plt.subplot2grid((2,2),(0,0))</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>以下两种写法是等价的：①ax=plt.figure(0)
+②ax=plt.subplot(2,1,1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>请画出函数f(x)=sin^2(x-2)e^(-x^2)在[0,2]区间的图像，并增加axis labels和title等图像信息。</t>
+  </si>
+  <si>
+    <t>设置坐标轴上下限</t>
+  </si>
+  <si>
+    <t>改变线条的颜色和粗细</t>
+  </si>
+  <si>
+    <t>调整图片大小</t>
+  </si>
+  <si>
+    <t>给特殊点做注释</t>
+  </si>
+  <si>
+    <t>BD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>从1到100所有数的总和为5050</t>
+  </si>
+  <si>
+    <t>ABCD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>done</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ID（uuid）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>passwd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>answer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>right</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wrong</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>逗号隔开题号</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>title</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>潘樾、郑南燕4、5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>以下关于字符串.strip()方法功能说明正确的是：</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>连接两个字符串序列</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>替换字符串中特定字符</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>去掉字符串两侧制定字符</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>按照指定字符分割字符串为数组</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -270,7 +562,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -288,6 +580,19 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -576,10 +881,10 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="3" customWidth="1"/>
     <col min="2" max="2" width="43.109375" style="4" customWidth="1"/>
@@ -611,8 +916,8 @@
       <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>2</v>
+      <c r="C2" s="7" t="s">
+        <v>6</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>11</v>
@@ -646,7 +951,7 @@
         <v>12</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>6</v>
+        <v>113</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>9</v>
@@ -662,8 +967,8 @@
       <c r="B5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>2</v>
+      <c r="C5" s="7" t="s">
+        <v>6</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>8</v>
@@ -714,6 +1019,9 @@
       </c>
       <c r="C10" s="9" t="s">
         <v>2</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -745,20 +1053,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAC84801-4A56-45D7-8C76-CF11C95D660A}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>114</v>
       </c>
       <c r="B1" t="s">
-        <v>22</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -766,7 +1074,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -774,7 +1082,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -782,7 +1090,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -790,7 +1098,15 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -801,81 +1117,204 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3167173-C41A-46D9-B764-711529E2D52A}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="82.8" x14ac:dyDescent="0.25">
+      <c r="A2" s="14">
+        <v>101</v>
+      </c>
+      <c r="B2" s="14">
+        <v>1</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="110.4" x14ac:dyDescent="0.25">
+      <c r="A3" s="14">
+        <v>102</v>
+      </c>
+      <c r="B3" s="14">
+        <v>1</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="110.4" x14ac:dyDescent="0.25">
+      <c r="A4" s="14">
+        <v>103</v>
+      </c>
+      <c r="B4" s="14">
+        <v>1</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="B1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="G4" s="14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="193.2" x14ac:dyDescent="0.25">
+      <c r="A5" s="14">
+        <v>104</v>
+      </c>
+      <c r="B5" s="14">
+        <v>1</v>
+      </c>
+      <c r="C5" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="F1" t="s">
+      <c r="D5" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="G1" t="s">
+      <c r="E5" s="14" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>101</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>102</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>103</v>
-      </c>
-      <c r="B4">
+      <c r="F5" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="96.6" x14ac:dyDescent="0.25">
+      <c r="A6" s="14">
+        <v>105</v>
+      </c>
+      <c r="B6" s="14">
         <v>3</v>
       </c>
-      <c r="C4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E4" t="s">
-        <v>28</v>
-      </c>
+      <c r="C6" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="165.6" x14ac:dyDescent="0.25">
+      <c r="A7" s="14">
+        <v>106</v>
+      </c>
+      <c r="B7" s="14">
+        <v>1</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="69" x14ac:dyDescent="0.25">
+      <c r="A8" s="14">
+        <v>107</v>
+      </c>
+      <c r="B8" s="14">
+        <v>5</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+    </row>
+    <row r="9" spans="1:7" ht="409.6" x14ac:dyDescent="0.25">
+      <c r="A9" s="14">
+        <v>108</v>
+      </c>
+      <c r="B9" s="14">
+        <v>5</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -885,76 +1324,171 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3754BF48-4712-4C5F-819B-44BEE3C566FB}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:E2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="B1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1" t="s">
+    <row r="1" spans="1:7" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="D1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="C1" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="138" x14ac:dyDescent="0.25">
+      <c r="A2" s="11">
         <v>201</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="B2" s="11">
+        <v>2</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="E2" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+    </row>
+    <row r="3" spans="1:7" ht="151.80000000000001" x14ac:dyDescent="0.25">
+      <c r="A3" s="11">
         <v>202</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="11">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="C3" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="E3" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+    </row>
+    <row r="4" spans="1:7" ht="69" x14ac:dyDescent="0.25">
+      <c r="A4" s="11">
         <v>203</v>
       </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E4" t="s">
-        <v>28</v>
-      </c>
+      <c r="B4" s="11">
+        <v>2</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="E4" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+    </row>
+    <row r="5" spans="1:7" ht="138" x14ac:dyDescent="0.25">
+      <c r="A5" s="11">
+        <v>204</v>
+      </c>
+      <c r="B5" s="11">
+        <v>1</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="165.6" x14ac:dyDescent="0.25">
+      <c r="A6" s="11">
+        <v>205</v>
+      </c>
+      <c r="B6" s="11">
+        <v>1</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D6" s="11">
+        <v>0</v>
+      </c>
+      <c r="E6" s="11">
+        <v>4</v>
+      </c>
+      <c r="F6" s="11">
+        <v>10</v>
+      </c>
+      <c r="G6" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="82.8" x14ac:dyDescent="0.25">
+      <c r="A7" s="11">
+        <v>206</v>
+      </c>
+      <c r="B7" s="11">
+        <v>4</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="D7" s="11">
+        <v>6</v>
+      </c>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+    </row>
+    <row r="8" spans="1:7" ht="207" x14ac:dyDescent="0.25">
+      <c r="A8" s="11">
+        <v>207</v>
+      </c>
+      <c r="B8" s="11">
+        <v>5</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -964,60 +1498,667 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF431F51-268F-41C7-AD62-8294863CF015}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:7" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="82.8" x14ac:dyDescent="0.25">
+      <c r="A2" s="11">
+        <v>301</v>
+      </c>
+      <c r="B2" s="11">
+        <v>2</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="E2" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+    </row>
+    <row r="3" spans="1:7" ht="110.4" x14ac:dyDescent="0.25">
+      <c r="A3" s="11">
+        <v>302</v>
+      </c>
+      <c r="B3" s="11">
+        <v>2</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="E3" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+    </row>
+    <row r="4" spans="1:7" ht="124.2" x14ac:dyDescent="0.25">
+      <c r="A4" s="11">
+        <v>303</v>
+      </c>
+      <c r="B4" s="11">
+        <v>2</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="D4" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="E4" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+    </row>
+    <row r="5" spans="1:7" ht="110.4" x14ac:dyDescent="0.25">
+      <c r="A5" s="11">
+        <v>304</v>
+      </c>
+      <c r="B5" s="11">
+        <v>1</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="110.4" x14ac:dyDescent="0.25">
+      <c r="A6" s="11">
+        <v>305</v>
+      </c>
+      <c r="B6" s="11">
+        <v>1</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="207" x14ac:dyDescent="0.25">
+      <c r="A7" s="11">
+        <v>306</v>
+      </c>
+      <c r="B7" s="11">
+        <v>1</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="96.6" x14ac:dyDescent="0.25">
+      <c r="A8" s="11">
+        <v>307</v>
+      </c>
+      <c r="B8" s="11">
+        <v>5</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB601933-D9FC-4DA0-ABB2-783CD8E1B6DF}">
-  <dimension ref="A1:B5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{833DFFC1-33CF-4487-9C2C-DAF397A8518B}">
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="138" x14ac:dyDescent="0.25">
+      <c r="A2" s="11">
+        <v>401</v>
+      </c>
+      <c r="B2" s="11">
+        <v>2</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="D2" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="E2" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+    </row>
+    <row r="3" spans="1:7" ht="96.6" x14ac:dyDescent="0.25">
+      <c r="A3" s="11">
+        <v>402</v>
+      </c>
+      <c r="B3" s="11">
+        <v>2</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D3" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="E3" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+    </row>
+    <row r="4" spans="1:7" ht="69" x14ac:dyDescent="0.25">
+      <c r="A4" s="11">
+        <v>403</v>
+      </c>
+      <c r="B4" s="11">
+        <v>3</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="151.80000000000001" x14ac:dyDescent="0.25">
+      <c r="A5" s="11">
+        <v>404</v>
+      </c>
+      <c r="B5" s="11">
+        <v>2</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="D5" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+    </row>
+    <row r="6" spans="1:7" ht="124.2" x14ac:dyDescent="0.25">
+      <c r="A6" s="11">
+        <v>405</v>
+      </c>
+      <c r="B6" s="11">
+        <v>2</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="D6" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="E6" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+    </row>
+    <row r="7" spans="1:7" ht="179.4" x14ac:dyDescent="0.25">
+      <c r="A7" s="11">
+        <v>406</v>
+      </c>
+      <c r="B7" s="11">
+        <v>5</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C73EC95-A5FF-4384-9B94-FFEB63EA5EB1}">
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB601933-D9FC-4DA0-ABB2-783CD8E1B6DF}">
+  <dimension ref="A1:C31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="C1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>101</v>
       </c>
-      <c r="B2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>102</v>
       </c>
-      <c r="B3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>103</v>
       </c>
-      <c r="B4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
+        <v>104</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>105</v>
+      </c>
+      <c r="C6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>106</v>
+      </c>
+      <c r="C7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
         <v>201</v>
+      </c>
+      <c r="C10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>202</v>
+      </c>
+      <c r="C11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>203</v>
+      </c>
+      <c r="C12" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>204</v>
+      </c>
+      <c r="C13" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>205</v>
+      </c>
+      <c r="C14" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>206</v>
+      </c>
+      <c r="C15">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>207</v>
+      </c>
+      <c r="C16" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>301</v>
+      </c>
+      <c r="C17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>302</v>
+      </c>
+      <c r="C18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>303</v>
+      </c>
+      <c r="C19" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>304</v>
+      </c>
+      <c r="C20" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>305</v>
+      </c>
+      <c r="C21" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>306</v>
+      </c>
+      <c r="C22" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>401</v>
+      </c>
+      <c r="C24" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>402</v>
+      </c>
+      <c r="C25" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>403</v>
+      </c>
+      <c r="C26" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>404</v>
+      </c>
+      <c r="C27" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>405</v>
+      </c>
+      <c r="C28" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>502</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04228AEB-9669-4AED-A5BB-C9A7C51969BC}">
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="9" max="9" width="16.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G1" t="s">
+        <v>106</v>
+      </c>
+      <c r="H1" t="s">
+        <v>107</v>
+      </c>
+      <c r="I1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D2" s="15">
+        <v>101102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>